<commit_message>
C2 2.2.8 Started and Initial writing added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="2.2.6 Information Access and" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -60,13 +60,54 @@
   </si>
   <si>
     <t>Tree Plantation</t>
+  </si>
+  <si>
+    <t>Remark/ any additional info</t>
+  </si>
+  <si>
+    <t>Government Residential Womens Polytechinc, Latur</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Format : List of information about </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t>Events/Activity</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Verdana"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> conducted for Womens/Students</t>
+    </r>
+  </si>
+  <si>
+    <t>Year : 2019-20</t>
+  </si>
+  <si>
+    <t>Year : 2018-19</t>
+  </si>
+  <si>
+    <t>Year : 2017-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +118,35 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
@@ -117,13 +187,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -417,92 +500,316 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:F10"/>
+  <dimension ref="B4:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="23.7109375" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:7" ht="19.5">
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="2:7" ht="19.5">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75">
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="1">
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="1">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="1">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="1">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9" s="1">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10" s="1">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="1">
+        <v>5</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="1">
+        <v>6</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="1">
+        <v>2</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="1">
+        <v>3</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="1">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="1">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="1">
+        <v>6</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B19:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial commit on 10 July SYNC Both ADA C6 and Fin_ADA
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -102,12 +102,87 @@
   <si>
     <t>Year : 2017-18</t>
   </si>
+  <si>
+    <t>Menstrual Hygiene management</t>
+  </si>
+  <si>
+    <t>Dr. Shilpa Tadurwar</t>
+  </si>
+  <si>
+    <t>Shajyog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shri. Akash Gholap </t>
+  </si>
+  <si>
+    <t>Karate training</t>
+  </si>
+  <si>
+    <t>13-23 December 2019</t>
+  </si>
+  <si>
+    <t>Shri. Datta Kadam, Japan Karate Association</t>
+  </si>
+  <si>
+    <t>Yog shibir</t>
+  </si>
+  <si>
+    <t>Karate Shibir phase II</t>
+  </si>
+  <si>
+    <t>MCM and diseases</t>
+  </si>
+  <si>
+    <t>महिला सुरक्षाविषयक कायदे</t>
+  </si>
+  <si>
+    <t>बाभळगाव पोलीस स्टेशन</t>
+  </si>
+  <si>
+    <t>Health Camp    ( blood test )</t>
+  </si>
+  <si>
+    <t>5th March 2020</t>
+  </si>
+  <si>
+    <t>Rotary club of India</t>
+  </si>
+  <si>
+    <t>11days - Feb 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motivation and time management </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logical Thinking </t>
+  </si>
+  <si>
+    <t>Pranayam and Yoga</t>
+  </si>
+  <si>
+    <t xml:space="preserve">महिलांवरील अत्याचारासंबंधी कायदे </t>
+  </si>
+  <si>
+    <t>Shri Raghunath A Kulkarni, PLGP Latur</t>
+  </si>
+  <si>
+    <t>Smt. V B Swami, V A I T Latur, Shri Avinash Jadhav and Shri Menkudle, MindLabz, Latur</t>
+  </si>
+  <si>
+    <t>Shri V B Mundhe, Patanjali Yogpeeth Latur</t>
+  </si>
+  <si>
+    <t>Shri. P M Makode, P.I, PTC Bhabhalgaon</t>
+  </si>
+  <si>
+    <t>Dr. Shilpa Tadurwar, Suman Industries, Latur</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +226,19 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,14 +287,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -500,53 +597,53 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:G36"/>
+  <dimension ref="B4:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.85546875" customWidth="1"/>
     <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -569,202 +666,258 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="1">
+      <c r="B11" s="8">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="3"/>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="1">
+      <c r="B12" s="8">
         <v>2</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="3"/>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="1">
+      <c r="B13" s="8">
         <v>3</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="3"/>
+      <c r="C13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="1">
+      <c r="B14" s="8">
         <v>4</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="3"/>
+      <c r="C14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="1">
+      <c r="B15" s="8">
         <v>5</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="1">
+      <c r="B16" s="8">
         <v>6</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="8">
+        <v>7</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="8">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="2" t="s">
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="1">
-        <v>3</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" ht="42" customHeight="1">
       <c r="B24" s="1">
-        <v>4</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" ht="21" customHeight="1">
       <c r="B25" s="1">
-        <v>5</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="2:7">
       <c r="B26" s="1">
-        <v>6</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>38</v>
+      </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="F26" s="1"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="7" t="s">
+    <row r="27" spans="2:7">
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="1">
+        <v>6</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-    </row>
-    <row r="30" spans="2:7">
-      <c r="B30" s="2" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="2:7">
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="2:7">
-      <c r="B32" s="1">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -774,7 +927,7 @@
     </row>
     <row r="34" spans="2:7">
       <c r="B34" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -784,7 +937,7 @@
     </row>
     <row r="35" spans="2:7">
       <c r="B35" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -794,7 +947,7 @@
     </row>
     <row r="36" spans="2:7">
       <c r="B36" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -802,13 +955,33 @@
       <c r="F36" s="1"/>
       <c r="G36" s="3"/>
     </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="1">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="1">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="C4:G4"/>
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
C2 Personality development cell data added in excel sheet
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="2.2.6 Information Access and" sheetId="1" r:id="rId1"/>
     <sheet name="2.2.7 Professional Skills" sheetId="2" r:id="rId2"/>
     <sheet name="2.2.8 Co-Curricular and Extra C" sheetId="3" r:id="rId3"/>
+    <sheet name="Personality develop. cell" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -177,12 +178,57 @@
   <si>
     <t>Dr. Shilpa Tadurwar, Suman Industries, Latur</t>
   </si>
+  <si>
+    <t xml:space="preserve">जीवन संजीवनी </t>
+  </si>
+  <si>
+    <t>Mr. Rajesh Chavhan, Founder of 'Jeevan Sanjiwani', Sahyadri Nagar, Wai Satara</t>
+  </si>
+  <si>
+    <t>74+</t>
+  </si>
+  <si>
+    <t>Career planning</t>
+  </si>
+  <si>
+    <t>Mr. Devichand Katariya, Career Consultant, Seed Management Services Ltd, Pune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Career opportunity </t>
+  </si>
+  <si>
+    <t>Dr. S G Kahalekar, Gramin College of Engineering, Nanded.(Siemens IT Solutions)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communication Skills </t>
+  </si>
+  <si>
+    <t>Mr. Sachidanandan Dhage</t>
+  </si>
+  <si>
+    <t>43+</t>
+  </si>
+  <si>
+    <t>Mr. Vivekanand Dhage and Mr. Sachidanandan Dhage</t>
+  </si>
+  <si>
+    <t>Personality development and Environmental issues</t>
+  </si>
+  <si>
+    <t>Dr. Prithaviraj S. Lucky, Gyan Chetana Charitable Trust, Bidar, Karnataka</t>
+  </si>
+  <si>
+    <t>Events under Personality development Cell : Mr Hasorikar sir / Shubhangi Shinde Mam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Experts Speak on Communication Skills development </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +285,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -275,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,6 +347,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,13 +365,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -599,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -614,13 +686,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
       <c r="C5" s="4"/>
@@ -630,20 +702,20 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -666,127 +738,127 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="8">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="8">
+      <c r="B12" s="5">
         <v>2</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8" t="s">
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="8">
+      <c r="B13" s="5">
         <v>3</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="8">
+      <c r="B14" s="5">
         <v>4</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="8">
+      <c r="B15" s="5">
         <v>5</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="8">
+      <c r="B16" s="5">
         <v>6</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="8">
+      <c r="B17" s="5">
         <v>7</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="8">
+      <c r="B18" s="5">
         <v>8</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
@@ -830,7 +902,7 @@
         <v>36</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F24" s="1"/>
@@ -854,7 +926,7 @@
       <c r="B26" s="1">
         <v>4</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D26" s="1"/>
@@ -868,11 +940,11 @@
       <c r="B27" s="1">
         <v>5</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="1"/>
@@ -889,11 +961,11 @@
       <c r="G28" s="3"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
@@ -993,7 +1065,7 @@
   <dimension ref="B3:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B3" sqref="B3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1106,4 +1178,154 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="C2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="22.5">
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43293</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="22.5">
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43154</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="2:6" ht="22.5">
+      <c r="B7" s="12">
+        <v>2</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43120</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="2:6" ht="33.75">
+      <c r="B8" s="12">
+        <v>6</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="13">
+        <v>43110</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="12">
+        <v>4</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="13">
+        <v>42984</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="33.75">
+      <c r="B10" s="12">
+        <v>5</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="13">
+        <v>42966</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="E16" s="1"/>
+    </row>
+  </sheetData>
+  <sortState ref="B5:F10">
+    <sortCondition descending="1" ref="D5:D10"/>
+  </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
C6 Webinar Faclility Images added , C6 Doc BSNL and Internet faclity added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -356,6 +356,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,15 +376,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,7 +649,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -686,13 +686,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
       <c r="C5" s="4"/>
@@ -702,20 +702,20 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -854,11 +854,11 @@
       <c r="G18" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
@@ -961,11 +961,11 @@
       <c r="G28" s="3"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
@@ -1197,12 +1197,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="2" t="s">
@@ -1222,98 +1222,98 @@
       </c>
     </row>
     <row r="5" spans="2:6" ht="22.5">
-      <c r="B5" s="12">
+      <c r="B5" s="8">
         <v>1</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="9">
         <v>43293</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="22.5">
-      <c r="B6" s="12">
+      <c r="B6" s="8">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="9">
         <v>43154</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="8"/>
     </row>
     <row r="7" spans="2:6" ht="22.5">
-      <c r="B7" s="12">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="9">
         <v>43120</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:6" ht="33.75">
-      <c r="B8" s="12">
+      <c r="B8" s="8">
         <v>6</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="9">
         <v>43110</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="8"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="12">
+      <c r="B9" s="8">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="9">
         <v>42984</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="33.75">
-      <c r="B10" s="12">
+      <c r="B10" s="8">
         <v>5</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="9">
         <v>42966</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="8"/>
     </row>
     <row r="16" spans="2:6">
       <c r="E16" s="1"/>

</xml_diff>

<commit_message>
C2 Activities adding in sheet started
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2.2.6 Information Access and" sheetId="1" r:id="rId1"/>
     <sheet name="2.2.7 Professional Skills" sheetId="2" r:id="rId2"/>
     <sheet name="2.2.8 Co-Curricular and Extra C" sheetId="3" r:id="rId3"/>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -222,6 +223,9 @@
   </si>
   <si>
     <t xml:space="preserve">Experts Speak on Communication Skills development </t>
+  </si>
+  <si>
+    <t>Name of the Event/Activity</t>
   </si>
 </sst>
 </file>
@@ -649,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -672,7 +676,7 @@
   <dimension ref="B4:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B9" sqref="B9:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1062,120 +1066,160 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:N10"/>
+  <dimension ref="B6:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14">
-      <c r="B3" s="2" t="s">
+    <row r="6" spans="2:14">
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+    </row>
+    <row r="7" spans="2:14">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="2:14">
+      <c r="B9" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="N9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
+      <c r="B10" s="5">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="N10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" s="5">
         <v>4</v>
       </c>
-      <c r="N3" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="N11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="N4" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="N12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="B13" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
-      <c r="B5" s="1">
-        <v>2</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="N5" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="N13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
+      <c r="B14" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="N6" t="s">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="N14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
+      <c r="B15" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="B7" s="1">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="N7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="1">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="N8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="1">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="N9" t="s">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="N15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
-      <c r="N10" t="s">
+    <row r="16" spans="2:14">
+      <c r="N16" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B6:D6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1184,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1328,4 +1372,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Initial Entries are added into excel sheet
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>Name of the Event/Activity</t>
+  </si>
+  <si>
+    <t>How to Write on Wikipedia in "Marathi Language"</t>
+  </si>
+  <si>
+    <t>Resource Person/Conducting authority</t>
+  </si>
+  <si>
+    <t>Intitute Level Activity</t>
+  </si>
+  <si>
+    <t>Mrs. A S Patil, Lecturer in Computer Engg, G.R.W.P Latur</t>
   </si>
 </sst>
 </file>
@@ -339,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +392,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,7 +671,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1069,13 +1087,13 @@
   <dimension ref="B6:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
@@ -1101,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>4</v>
@@ -1110,15 +1128,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" ht="25.5">
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="C8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="15">
+        <v>43843</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="5">
+        <v>61</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="2:14">
       <c r="B9" s="5">

</xml_diff>

<commit_message>
Quiz and Poster competition added in excel sheet
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -238,6 +238,39 @@
   </si>
   <si>
     <t>Mrs. A S Patil, Lecturer in Computer Engg, G.R.W.P Latur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mrs.S A Agarkar, Chief Coordinator ECO CLUB and Lecturer in ET, Smt. R D Kasar, Lecturer in Computer Engg. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree Plantation Activity at Village Nagzari </t>
+  </si>
+  <si>
+    <t>Technical Poster Presentation on Topics a) Data Mining b) Internet of Things c) Cyber Security d) Artificial Intelligence e) Green Computing f) Save water Save Life</t>
+  </si>
+  <si>
+    <t>Program Level Activity</t>
+  </si>
+  <si>
+    <t>Blind Programming competition on C++ Language</t>
+  </si>
+  <si>
+    <t>Blind Programming competition on JAVA Language</t>
+  </si>
+  <si>
+    <t>Quiz Competition on "C Programming"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 180+ (CO1I,CO3I,CO5I)</t>
+  </si>
+  <si>
+    <t>66+(CO3I)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 50+(CO5I)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66+(CO3I)</t>
   </si>
 </sst>
 </file>
@@ -351,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -381,6 +414,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -393,10 +429,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -671,7 +707,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -708,13 +744,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
       <c r="C5" s="4"/>
@@ -724,20 +760,20 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -876,11 +912,11 @@
       <c r="G18" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
@@ -983,11 +1019,11 @@
       <c r="G28" s="3"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
@@ -1087,7 +1123,7 @@
   <dimension ref="B6:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1102,139 +1138,189 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:14">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="25.5">
-      <c r="B8" s="5">
+      <c r="B8" s="11">
         <v>1</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="17">
         <v>43843</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="11">
         <v>61</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
-      <c r="B9" s="5">
+    <row r="9" spans="2:14" ht="38.25">
+      <c r="B9" s="11">
         <v>2</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="C9" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="17">
+        <v>43864</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="11">
+        <v>15</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="N9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
-      <c r="B10" s="5">
+    <row r="10" spans="2:14" ht="51">
+      <c r="B10" s="11">
         <v>3</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="C10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="17">
+        <v>43726</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
-      <c r="B11" s="5">
+    <row r="11" spans="2:14" ht="25.5">
+      <c r="B11" s="11">
         <v>4</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="C11" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="17">
+        <v>43721</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="5">
+    <row r="12" spans="2:14" ht="25.5">
+      <c r="B12" s="11">
         <v>5</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="C12" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="17">
+        <v>43712</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
-      <c r="B13" s="5">
+    <row r="13" spans="2:14" ht="25.5">
+      <c r="B13" s="11">
         <v>6</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="C13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="17">
+        <v>43704</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>67</v>
+      </c>
       <c r="N13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="5">
+      <c r="B14" s="11">
         <v>7</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
       <c r="N14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="5">
+      <c r="B15" s="11">
         <v>8</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
       <c r="N15" t="s">
         <v>11</v>
       </c>
@@ -1269,12 +1355,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
C2 AY 2018-19 Activity added till RA Kulkarni Page 05 07 18
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -271,6 +271,66 @@
   </si>
   <si>
     <t xml:space="preserve"> 66+(CO3I)</t>
+  </si>
+  <si>
+    <t>Head of Computer Engg department</t>
+  </si>
+  <si>
+    <t>Blind Programming competition on C Language</t>
+  </si>
+  <si>
+    <t>Swachhata Abhiyan (Cleanliness Program)</t>
+  </si>
+  <si>
+    <t>Technical Poster Presentation on Topics a) Internet Security b) Artificial Intelligence c) Robotics computing d) Social Media Awareness e) Latest technologies in computer science f) E-Waste recycling</t>
+  </si>
+  <si>
+    <t>वेळेचे सुव्यवस्थापन (Time Management)</t>
+  </si>
+  <si>
+    <t>तार्किक विचार (Logical Thinking)</t>
+  </si>
+  <si>
+    <t>आहार आणि स्वास्थ्य ( Diet and Health)</t>
+  </si>
+  <si>
+    <t>सखोल ध्यान (Deep meditation)</t>
+  </si>
+  <si>
+    <t>प्राणायाम आणि योग (Pranayama and Yoga)</t>
+  </si>
+  <si>
+    <t>स्व-संरक्षण (Self Protection)</t>
+  </si>
+  <si>
+    <t>आजची राष्ट्रभक्ती (Today's Patriotism)</t>
+  </si>
+  <si>
+    <t>20-09-2018 to 26-09-2018</t>
+  </si>
+  <si>
+    <t>Quiz  Trainers GRWP Latur</t>
+  </si>
+  <si>
+    <t>Professinal from Medical field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ब्रम्हकुमारी आश्रम / मनः शक्ती केंद्र </t>
+  </si>
+  <si>
+    <t>Yoga Teacher</t>
+  </si>
+  <si>
+    <t>Smt Ashwini Taak</t>
+  </si>
+  <si>
+    <t>Social Worker-NGO</t>
+  </si>
+  <si>
+    <t>Shri. Raghunath Ananat Kulkarni - Expert from management field</t>
+  </si>
+  <si>
+    <t>70+</t>
   </si>
 </sst>
 </file>
@@ -349,12 +409,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -384,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -417,6 +483,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,11 +501,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,7 +779,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -744,13 +816,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
       <c r="C5" s="4"/>
@@ -760,20 +832,20 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -912,11 +984,11 @@
       <c r="G18" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
@@ -1019,11 +1091,11 @@
       <c r="G28" s="3"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="12" t="s">
+      <c r="B31" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
@@ -1120,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B6:N16"/>
+  <dimension ref="B6:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1138,29 +1210,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:14">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1171,7 +1243,7 @@
       <c r="C8" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="13">
         <v>43843</v>
       </c>
       <c r="E8" s="11" t="s">
@@ -1191,7 +1263,7 @@
       <c r="C9" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="13">
         <v>43864</v>
       </c>
       <c r="E9" s="11" t="s">
@@ -1214,7 +1286,7 @@
       <c r="C10" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <v>43726</v>
       </c>
       <c r="E10" s="11" t="s">
@@ -1237,7 +1309,7 @@
       <c r="C11" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="13">
         <v>43721</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -1260,7 +1332,7 @@
       <c r="C12" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="13">
         <v>43712</v>
       </c>
       <c r="E12" s="11" t="s">
@@ -1283,7 +1355,7 @@
       <c r="C13" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="13">
         <v>43704</v>
       </c>
       <c r="E13" s="11" t="s">
@@ -1330,11 +1402,269 @@
         <v>12</v>
       </c>
     </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="13">
+        <v>43342</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="11">
+        <v>58</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="25.5">
+      <c r="B21" s="11">
+        <v>2</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="13">
+        <v>43364</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" s="11">
+        <v>15</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="25.5">
+      <c r="B22" s="11">
+        <v>3</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="13">
+        <v>43355</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="11">
+        <v>15</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="63.75">
+      <c r="B23" s="11">
+        <v>4</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="13">
+        <v>43370</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="25.5">
+      <c r="B24" s="11">
+        <v>5</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="13">
+        <v>43286</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="11">
+        <v>6</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" s="13">
+        <v>43307</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="11">
+        <v>7</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13">
+        <v>43321</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="11">
+        <v>8</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="13">
+        <v>43335</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="11">
+        <v>9</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D28" s="13">
+        <v>43349</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="25.5">
+      <c r="B29" s="11">
+        <v>10</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="11">
+        <v>11</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" s="13">
+        <v>43377</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="11">
+        <v>12</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="19"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1355,12 +1685,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
Data from AM 16-17 and 17-18 added and reference files also added
</commit_message>
<xml_diff>
--- a/C2/C2 NBA.xlsx
+++ b/C2/C2 NBA.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15390" windowHeight="8670" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="2.2.6 Information Access and" sheetId="1" r:id="rId1"/>
     <sheet name="2.2.7 Professional Skills" sheetId="2" r:id="rId2"/>
     <sheet name="2.2.8 Co-Curricular and Extra C" sheetId="3" r:id="rId3"/>
     <sheet name="Personality develop. cell" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="List of Certificate" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
   <si>
     <t xml:space="preserve">Sr.No </t>
   </si>
@@ -489,6 +489,9 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,13 +501,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:G18"/>
+    <sheetView topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -816,13 +816,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:7" ht="19.5">
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="2:7" ht="19.5">
       <c r="C5" s="4"/>
@@ -832,20 +832,20 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="2:7" ht="15.75">
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
@@ -984,11 +984,11 @@
       <c r="G18" s="5"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
@@ -1091,11 +1091,11 @@
       <c r="G28" s="3"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
     </row>
     <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B6:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1656,7 +1656,7 @@
       <c r="G32" s="11"/>
     </row>
     <row r="33" spans="3:3">
-      <c r="C33" s="19"/>
+      <c r="C33" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1672,7 +1672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1685,12 +1685,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="2" t="s">
@@ -1820,12 +1820,95 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="C2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8" s="8"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="8"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="E16" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>